<commit_message>
Adjust leidingweerstand to use package
</commit_message>
<xml_diff>
--- a/productiecapaciteit/data/strang_props6.xlsx
+++ b/productiecapaciteit/data/strang_props6.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tombb\OneDrive - PWN\Documenten\PTCAP ICAS 2021\P300 analyse\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tombb\Python scripts\python-pwn-productiecapaciteit-infiltratiegebieden\productiecapaciteit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029FE18A-5C9B-4939-84FA-4FCFCE8E4CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB4CB2D-B319-446B-837F-32CB1C73CBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15615" yWindow="3330" windowWidth="21600" windowHeight="14625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="215">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -507,6 +508,177 @@
   </si>
   <si>
     <t>put_a_slope</t>
+  </si>
+  <si>
+    <t>(2015, (35, 37))</t>
+  </si>
+  <si>
+    <t>(2015, (43, 44))</t>
+  </si>
+  <si>
+    <t>(2015, (45, 47))</t>
+  </si>
+  <si>
+    <t>(2015, (48, 49))</t>
+  </si>
+  <si>
+    <t>(2015, (50, 51))</t>
+  </si>
+  <si>
+    <t>(2015, (7, 8))</t>
+  </si>
+  <si>
+    <t>(2016, (38, 39))</t>
+  </si>
+  <si>
+    <t>(2016, (40, 42))</t>
+  </si>
+  <si>
+    <t>(2016, (44, 45))</t>
+  </si>
+  <si>
+    <t>(2016, (48, 49))</t>
+  </si>
+  <si>
+    <t>(2017, (5, 6))</t>
+  </si>
+  <si>
+    <t>(2017, 8, 10)</t>
+  </si>
+  <si>
+    <t>(2017, 11, 12)</t>
+  </si>
+  <si>
+    <t>(2017, 36, 37)</t>
+  </si>
+  <si>
+    <t>(2017, 40, 41)</t>
+  </si>
+  <si>
+    <t>(2017, 43, 45)</t>
+  </si>
+  <si>
+    <t>(2017, 46, 47)</t>
+  </si>
+  <si>
+    <t>(2017, 50, 51)</t>
+  </si>
+  <si>
+    <t>(2018, 3, 4)</t>
+  </si>
+  <si>
+    <t>(2018, 6, 7)</t>
+  </si>
+  <si>
+    <t>(2018, 10, 11)</t>
+  </si>
+  <si>
+    <t>(2018, 36, 38)</t>
+  </si>
+  <si>
+    <t>(2018, 41, 42)</t>
+  </si>
+  <si>
+    <t>(2018, 44, 45)</t>
+  </si>
+  <si>
+    <t>(2018, 47, 48)</t>
+  </si>
+  <si>
+    <t>(2018, 49, 51)</t>
+  </si>
+  <si>
+    <t>(2019, 2, 3)</t>
+  </si>
+  <si>
+    <t>(2019, 6, 7)</t>
+  </si>
+  <si>
+    <t>(2019, 10, 11)</t>
+  </si>
+  <si>
+    <t>(2019, 36, 38)</t>
+  </si>
+  <si>
+    <t>(2019, 41, 42)</t>
+  </si>
+  <si>
+    <t>(2019, 44, 45)</t>
+  </si>
+  <si>
+    <t>(2019, 47, 48)</t>
+  </si>
+  <si>
+    <t>(2019, 49, 49)</t>
+  </si>
+  <si>
+    <t>(2020, 2, 3)</t>
+  </si>
+  <si>
+    <t>(2020, 6, 6)</t>
+  </si>
+  <si>
+    <t>(2020, 10, 11)</t>
+  </si>
+  <si>
+    <t>(2020, 31, 32)</t>
+  </si>
+  <si>
+    <t>(2020, 36, 37)</t>
+  </si>
+  <si>
+    <t>(2020, 39, 41)</t>
+  </si>
+  <si>
+    <t>(2020, 43, 44)</t>
+  </si>
+  <si>
+    <t>(2020, 48, 49)</t>
+  </si>
+  <si>
+    <t>(2020, 49, 50)</t>
+  </si>
+  <si>
+    <t>(2021, 1, 1)</t>
+  </si>
+  <si>
+    <t>(2021, 4, 8)</t>
+  </si>
+  <si>
+    <t>(2021, 9, 9)</t>
+  </si>
+  <si>
+    <t>(2021, 10, 11)</t>
+  </si>
+  <si>
+    <t>(2021, 13, 13)</t>
+  </si>
+  <si>
+    <t>(2020, 46, 46)</t>
+  </si>
+  <si>
+    <t>(2022, 35, 36)</t>
+  </si>
+  <si>
+    <t>(2022, 41, 42)</t>
+  </si>
+  <si>
+    <t>(2022, 47, 49)</t>
+  </si>
+  <si>
+    <t>(2022, 50, 51)</t>
+  </si>
+  <si>
+    <t>(2023, 1, 2)</t>
+  </si>
+  <si>
+    <t>(2023, 4, 5)</t>
+  </si>
+  <si>
+    <t>(2023, 7, 8)</t>
+  </si>
+  <si>
+    <t>(2023, 10, 13)</t>
   </si>
 </sst>
 </file>
@@ -525,6 +697,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -872,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3428,99 +3601,99 @@
         <v>117</v>
       </c>
       <c r="B35" t="str">
-        <f>B33 &amp; "_PT10 / 10 + " &amp; +B29-B30</f>
+        <f t="shared" ref="B35:Y35" si="0">B33 &amp; "_PT10 / 10 + " &amp; +B29-B30</f>
         <v>CAWQ01_PT10 / 10 + -0.25</v>
       </c>
       <c r="C35" t="str">
-        <f>C33 &amp; "_PT10 / 10 + " &amp; +C29-C30</f>
+        <f t="shared" si="0"/>
         <v>CAWQ02_PT10 / 10 + 0.08</v>
       </c>
       <c r="D35" t="str">
-        <f>D33 &amp; "_PT10 / 10 + " &amp; +D29-D30</f>
+        <f t="shared" si="0"/>
         <v>CAWQ03_PT10 / 10 + 0.11</v>
       </c>
       <c r="E35" t="str">
-        <f>E33 &amp; "_PT10 / 10 + " &amp; +E29-E30</f>
+        <f t="shared" si="0"/>
         <v>CAWQ04_PT10 / 10 + 0.1</v>
       </c>
       <c r="F35" t="str">
-        <f>F33 &amp; "_PT10 / 10 + " &amp; +F29-F30</f>
+        <f t="shared" si="0"/>
         <v>CAWQ05_PT10 / 10 + -0.16</v>
       </c>
       <c r="G35" t="str">
-        <f>G33 &amp; "_PT10 / 10 + " &amp; +G29-G30</f>
+        <f t="shared" si="0"/>
         <v>CAWQ06_PT10 / 10 + -0.08</v>
       </c>
       <c r="H35" t="str">
-        <f>H33 &amp; "_PT10 / 10 + " &amp; +H29-H30</f>
+        <f t="shared" si="0"/>
         <v>CAWP01_PT10 / 10 + -0.44</v>
       </c>
       <c r="I35" t="str">
-        <f>I33 &amp; "_PT10 / 10 + " &amp; +I29-I30</f>
+        <f t="shared" si="0"/>
         <v>CAWP02_PT10 / 10 + -0.47</v>
       </c>
       <c r="J35" t="str">
-        <f>J33 &amp; "_PT10 / 10 + " &amp; +J29-J30</f>
+        <f t="shared" si="0"/>
         <v>CAWP03_PT10 / 10 + -0.12</v>
       </c>
       <c r="K35" t="str">
-        <f>K33 &amp; "_PT10 / 10 + " &amp; +K29-K30</f>
+        <f t="shared" si="0"/>
         <v>CAWP04_PT10 / 10 + -0.2</v>
       </c>
       <c r="L35" t="str">
-        <f>L33 &amp; "_PT10 / 10 + " &amp; +L29-L30</f>
+        <f t="shared" si="0"/>
         <v>CAWP05_PT10 / 10 + 0.0200000000000001</v>
       </c>
       <c r="M35" t="str">
-        <f>M33 &amp; "_PT10 / 10 + " &amp; +M29-M30</f>
+        <f t="shared" si="0"/>
         <v>CAWP06_PT10 / 10 + -0.18</v>
       </c>
       <c r="N35" t="str">
-        <f>N33 &amp; "_PT10 / 10 + " &amp; +N29-N30</f>
+        <f t="shared" si="0"/>
         <v>HEW901_PT10 / 10 + 6.22</v>
       </c>
       <c r="O35" t="str">
-        <f>O33 &amp; "_PT10 / 10 + " &amp; +O29-O30</f>
+        <f t="shared" si="0"/>
         <v>HEW902_PT10 / 10 + 5.2</v>
       </c>
       <c r="P35" t="str">
-        <f>P33 &amp; "_PT10 / 10 + " &amp; +P29-P30</f>
+        <f t="shared" si="0"/>
         <v>HEW903_PT10 / 10 + 4.83</v>
       </c>
       <c r="Q35" t="str">
-        <f>Q33 &amp; "_PT10 / 10 + " &amp; +Q29-Q30</f>
+        <f t="shared" si="0"/>
         <v>HEW904_PT10 / 10 + 7.14</v>
       </c>
       <c r="R35" t="str">
-        <f>R33 &amp; "_PT10 / 10 + " &amp; +R29-R30</f>
+        <f t="shared" si="0"/>
         <v>HEW905_PT10 / 10 + 4.87</v>
       </c>
       <c r="S35" t="str">
-        <f>S33 &amp; "_PT10 / 10 + " &amp; +S29-S30</f>
+        <f t="shared" si="0"/>
         <v>HEW906_PT10 / 10 + 7.51</v>
       </c>
       <c r="T35" t="str">
-        <f>T33 &amp; "_PT10 / 10 + " &amp; +T29-T30</f>
+        <f t="shared" si="0"/>
         <v>HEW101_PT10 / 10 + 8.03</v>
       </c>
       <c r="U35" t="str">
-        <f>U33 &amp; "_PT10 / 10 + " &amp; +U29-U30</f>
+        <f t="shared" si="0"/>
         <v>HEW102_PT10 / 10 + 8.04</v>
       </c>
       <c r="V35" t="str">
-        <f>V33 &amp; "_PT10 / 10 + " &amp; +V29-V30</f>
+        <f t="shared" si="0"/>
         <v>HEW103_PT10 / 10 + 5.27</v>
       </c>
       <c r="W35" t="str">
-        <f>W33 &amp; "_PT10 / 10 + " &amp; +W29-W30</f>
+        <f t="shared" si="0"/>
         <v>HEW104_PT10 / 10 + 7.34</v>
       </c>
       <c r="X35" t="str">
-        <f>X33 &amp; "_PT10 / 10 + " &amp; +X29-X30</f>
+        <f t="shared" si="0"/>
         <v>HEW105_PT10 / 10 + 6.92</v>
       </c>
       <c r="Y35" t="str">
-        <f>Y33 &amp; "_PT10 / 10 + " &amp; +Y29-Y30</f>
+        <f t="shared" si="0"/>
         <v>HEW106_PT10 / 10 + 8.25</v>
       </c>
     </row>
@@ -3915,21 +4088,327 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fc8400a0-1a4f-4a7a-b485-adeb34e513bd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59AB176E-27A4-4AEF-B4A1-CFE70075B06B}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>197</v>
+      </c>
+      <c r="C12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" t="s">
+        <v>201</v>
+      </c>
+      <c r="D21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" t="s">
+        <v>178</v>
+      </c>
+      <c r="D22" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>166</v>
+      </c>
+      <c r="C23" t="s">
+        <v>205</v>
+      </c>
+      <c r="D23" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>168</v>
+      </c>
+      <c r="C24" t="s">
+        <v>185</v>
+      </c>
+      <c r="D24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fc8400a0-1a4f-4a7a-b485-adeb34e513bd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4168,6 +4647,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD85D50E-4653-4992-BCE8-249F2A1C10E6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BADBF8A8-0E22-4206-B90E-29320953DE1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4180,14 +4667,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD85D50E-4653-4992-BCE8-249F2A1C10E6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Minor adjustments. Losses report working and final modelparameters
</commit_message>
<xml_diff>
--- a/productiecapaciteit/data/strang_props6.xlsx
+++ b/productiecapaciteit/data/strang_props6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tombb\Python scripts\python-pwn-productiecapaciteit-infiltratiegebieden\productiecapaciteit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB4CB2D-B319-446B-837F-32CB1C73CBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86706827-AD71-4E7C-B68B-14F84404223F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14970" yWindow="4740" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="227">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -679,6 +679,42 @@
   </si>
   <si>
     <t>(2023, 10, 13)</t>
+  </si>
+  <si>
+    <t>(2021, 35, 36)</t>
+  </si>
+  <si>
+    <t>(2021, 38, 39)</t>
+  </si>
+  <si>
+    <t>(2021, 43, 44)</t>
+  </si>
+  <si>
+    <t>(2021, 43, 50)</t>
+  </si>
+  <si>
+    <t>(2021, 49, 50)</t>
+  </si>
+  <si>
+    <t>(2022, 1, 2)</t>
+  </si>
+  <si>
+    <t>(2022, 4, 5)</t>
+  </si>
+  <si>
+    <t>(2022, 7, 8)</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t xml:space="preserve">": </t>
+  </si>
+  <si>
+    <t>],</t>
+  </si>
+  <si>
+    <t>"</t>
   </si>
 </sst>
 </file>
@@ -735,12 +771,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1045,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y45"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:Y1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,7 +1565,7 @@
         <v>-2.48E-5</v>
       </c>
       <c r="C7" s="2">
-        <v>-2.5000000000000001E-5</v>
+        <v>-1.0000000000000001E-5</v>
       </c>
       <c r="D7" s="2">
         <v>-6.0000000000000002E-6</v>
@@ -1541,13 +1580,13 @@
         <v>-5.0000000000000001E-4</v>
       </c>
       <c r="H7" s="2">
-        <v>-1.7000000000000001E-4</v>
+        <v>-2.9999999999999997E-4</v>
       </c>
       <c r="I7" s="2">
         <v>-5.0000000000000004E-6</v>
       </c>
       <c r="J7" s="2">
-        <v>-2.3699999999999999E-4</v>
+        <v>-3.5E-4</v>
       </c>
       <c r="K7" s="2">
         <v>-5.0000000000000004E-6</v>
@@ -4090,328 +4129,624 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59AB176E-27A4-4AEF-B4A1-CFE70075B06B}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="A1:J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E2" t="s">
         <v>167</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="J2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" t="s">
         <v>171</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="J3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E4" t="s">
         <v>169</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>196</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="J4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" t="s">
         <v>159</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>180</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>188</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="J5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" t="s">
         <v>158</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="G6" t="s">
+        <v>217</v>
+      </c>
+      <c r="J6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D7" t="s">
+        <v>223</v>
+      </c>
+      <c r="E7" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="J7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" t="s">
+        <v>223</v>
+      </c>
+      <c r="E8" t="s">
         <v>165</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
         <v>181</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="H8" t="s">
+        <v>219</v>
+      </c>
+      <c r="J8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" t="s">
+        <v>223</v>
+      </c>
+      <c r="E9" t="s">
         <v>160</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>174</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>179</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="I9" t="s">
+        <v>216</v>
+      </c>
+      <c r="J9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E10" t="s">
         <v>162</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
         <v>182</v>
       </c>
-      <c r="D10" t="s">
+      <c r="G10" t="s">
         <v>190</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="J10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E11" t="s">
         <v>163</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
         <v>183</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="J11" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D12" t="s">
+        <v>223</v>
+      </c>
+      <c r="E12" t="s">
         <v>197</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="J12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>226</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D13" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" t="s">
         <v>175</v>
       </c>
-      <c r="C13" t="s">
+      <c r="F13" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="J13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>226</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E14" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="J14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D15" t="s">
+        <v>223</v>
+      </c>
+      <c r="E15" t="s">
         <v>186</v>
       </c>
-      <c r="C15" t="s">
+      <c r="F15" t="s">
         <v>194</v>
       </c>
-      <c r="D15" t="s">
+      <c r="G15" t="s">
+        <v>220</v>
+      </c>
+      <c r="H15" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="J15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D16" t="s">
+        <v>223</v>
+      </c>
+      <c r="E16" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="F16" t="s">
+        <v>222</v>
+      </c>
+      <c r="J16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>226</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D17" t="s">
+        <v>223</v>
+      </c>
+      <c r="E17" t="s">
         <v>170</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
         <v>184</v>
       </c>
-      <c r="D17" t="s">
+      <c r="G17" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="J17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>226</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D18" t="s">
+        <v>223</v>
+      </c>
+      <c r="E18" t="s">
         <v>164</v>
       </c>
-      <c r="C18" t="s">
+      <c r="F18" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="J18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>226</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D19" t="s">
+        <v>223</v>
+      </c>
+      <c r="E19" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="F19" t="s">
+        <v>221</v>
+      </c>
+      <c r="J19" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>226</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D20" t="s">
+        <v>223</v>
+      </c>
+      <c r="E20" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="F20" t="s">
+        <v>218</v>
+      </c>
+      <c r="J20" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>226</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D21" t="s">
+        <v>223</v>
+      </c>
+      <c r="E21" t="s">
         <v>177</v>
       </c>
-      <c r="C21" t="s">
+      <c r="F21" t="s">
         <v>201</v>
       </c>
-      <c r="D21" t="s">
+      <c r="G21" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="J21" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>226</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D22" t="s">
+        <v>223</v>
+      </c>
+      <c r="E22" t="s">
         <v>161</v>
       </c>
-      <c r="C22" t="s">
+      <c r="F22" t="s">
         <v>178</v>
       </c>
-      <c r="D22" t="s">
+      <c r="G22" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="J22" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>226</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D23" t="s">
+        <v>223</v>
+      </c>
+      <c r="E23" t="s">
         <v>166</v>
       </c>
-      <c r="C23" t="s">
+      <c r="F23" t="s">
         <v>205</v>
       </c>
-      <c r="D23" t="s">
+      <c r="G23" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="J23" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>226</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D24" t="s">
+        <v>223</v>
+      </c>
+      <c r="E24" t="s">
         <v>168</v>
       </c>
-      <c r="C24" t="s">
+      <c r="F24" t="s">
         <v>185</v>
       </c>
-      <c r="D24" t="s">
+      <c r="G24" t="s">
         <v>193</v>
+      </c>
+      <c r="J24" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fc8400a0-1a4f-4a7a-b485-adeb34e513bd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010081BE85D0812D9240B3A14D4E86FBD526" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="844c5fe439c283c57054fe603be8f4f0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fc8400a0-1a4f-4a7a-b485-adeb34e513bd" xmlns:ns4="f8e76daf-932e-4eb3-bd51-a2b94da941c5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5bfb24005f79649d2d34abed6e4c7d87" ns3:_="" ns4:_="">
     <xsd:import namespace="fc8400a0-1a4f-4a7a-b485-adeb34e513bd"/>
@@ -4646,10 +4981,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fc8400a0-1a4f-4a7a-b485-adeb34e513bd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD85D50E-4653-4992-BCE8-249F2A1C10E6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17420F09-E15D-430F-A548-6FE9174B4D1D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fc8400a0-1a4f-4a7a-b485-adeb34e513bd"/>
+    <ds:schemaRef ds:uri="f8e76daf-932e-4eb3-bd51-a2b94da941c5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4672,20 +5035,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17420F09-E15D-430F-A548-6FE9174B4D1D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD85D50E-4653-4992-BCE8-249F2A1C10E6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fc8400a0-1a4f-4a7a-b485-adeb34e513bd"/>
-    <ds:schemaRef ds:uri="f8e76daf-932e-4eb3-bd51-a2b94da941c5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added transient impulse responses
</commit_message>
<xml_diff>
--- a/productiecapaciteit/data/strang_props6.xlsx
+++ b/productiecapaciteit/data/strang_props6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tombb\Python scripts\python-pwn-productiecapaciteit-infiltratiegebieden\productiecapaciteit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E63A1F1-A18F-49C9-9CD0-307700334837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3817DD0B-548A-4191-981F-326D35451C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="247">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -721,13 +721,67 @@
   </si>
   <si>
     <t>Qmin_inzetvolgorde20230523</t>
+  </si>
+  <si>
+    <t>Inzetvolgorde</t>
+  </si>
+  <si>
+    <t>SOM</t>
+  </si>
+  <si>
+    <t>Som excl P400 &amp; Q500</t>
+  </si>
+  <si>
+    <t>Cap. test sep. '22</t>
+  </si>
+  <si>
+    <t>dx_tussenputten</t>
+  </si>
+  <si>
+    <t>[(-1, 75)]</t>
+  </si>
+  <si>
+    <t>[(-1, 250), (-1, 82)]</t>
+  </si>
+  <si>
+    <t>[(-2, 82)]</t>
+  </si>
+  <si>
+    <t>[(-2, 77)]</t>
+  </si>
+  <si>
+    <t>[(-2, 73)]</t>
+  </si>
+  <si>
+    <t>[(-1, 92)]</t>
+  </si>
+  <si>
+    <t>dx_mirrorwell</t>
+  </si>
+  <si>
+    <t>[(-1, 65)]</t>
+  </si>
+  <si>
+    <t>[(-2, 45)]</t>
+  </si>
+  <si>
+    <t>[(-2, 50)]</t>
+  </si>
+  <si>
+    <t>[(-2, 44)]</t>
+  </si>
+  <si>
+    <t>[(-2, 49)]</t>
+  </si>
+  <si>
+    <t>[(-1, 40)]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -741,6 +795,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -750,7 +810,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -773,11 +833,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -785,6 +865,16 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1088,10 +1178,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y47"/>
+  <dimension ref="A1:Y46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="T45" sqref="T45:Y46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2261,22 +2354,22 @@
         <v>51</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>3.37</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>2.83</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>2.92</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>2.93</v>
       </c>
       <c r="F16">
-        <v>2</v>
+        <v>2.94</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>3.77</v>
       </c>
       <c r="H16">
         <v>3.29</v>
@@ -2297,40 +2390,40 @@
         <v>3.17</v>
       </c>
       <c r="N16">
-        <v>4.5</v>
+        <v>5.04</v>
       </c>
       <c r="O16">
-        <v>4.5</v>
+        <v>6.2</v>
       </c>
       <c r="P16">
-        <v>4.5</v>
+        <v>6.12</v>
       </c>
       <c r="Q16">
-        <v>4.5</v>
+        <v>6.12</v>
       </c>
       <c r="R16">
-        <v>4.5</v>
+        <v>6.13</v>
       </c>
       <c r="S16">
-        <v>4.5</v>
+        <v>6.75</v>
       </c>
       <c r="T16">
-        <v>4.5</v>
+        <v>5.25</v>
       </c>
       <c r="U16">
-        <v>4.5</v>
+        <v>6.2</v>
       </c>
       <c r="V16">
-        <v>4.5</v>
+        <v>6.11</v>
       </c>
       <c r="W16">
-        <v>4.5</v>
+        <v>6.09</v>
       </c>
       <c r="X16">
-        <v>4.5</v>
+        <v>6.19</v>
       </c>
       <c r="Y16">
-        <v>4.5</v>
+        <v>6.23</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
@@ -4255,31 +4348,159 @@
         <v>673</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
-      <c r="Q47" s="2"/>
-      <c r="R47" s="2"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="2"/>
-      <c r="U47" s="2"/>
-      <c r="V47" s="2"/>
-      <c r="W47" s="2"/>
-      <c r="X47" s="2"/>
-      <c r="Y47" s="2"/>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B45">
+        <v>15</v>
+      </c>
+      <c r="C45">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>10</v>
+      </c>
+      <c r="E45">
+        <v>10</v>
+      </c>
+      <c r="F45">
+        <v>10</v>
+      </c>
+      <c r="G45">
+        <v>15</v>
+      </c>
+      <c r="H45">
+        <v>15</v>
+      </c>
+      <c r="I45">
+        <v>15</v>
+      </c>
+      <c r="J45">
+        <v>10</v>
+      </c>
+      <c r="K45">
+        <v>10</v>
+      </c>
+      <c r="L45">
+        <v>10</v>
+      </c>
+      <c r="M45">
+        <v>15</v>
+      </c>
+      <c r="N45">
+        <v>15</v>
+      </c>
+      <c r="O45">
+        <v>15</v>
+      </c>
+      <c r="P45">
+        <v>15</v>
+      </c>
+      <c r="Q45">
+        <v>15</v>
+      </c>
+      <c r="R45">
+        <v>15</v>
+      </c>
+      <c r="S45">
+        <v>45</v>
+      </c>
+      <c r="T45">
+        <v>15</v>
+      </c>
+      <c r="U45">
+        <v>15</v>
+      </c>
+      <c r="V45">
+        <v>15</v>
+      </c>
+      <c r="W45">
+        <v>15</v>
+      </c>
+      <c r="X45">
+        <v>15</v>
+      </c>
+      <c r="Y45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B46" t="s">
+        <v>234</v>
+      </c>
+      <c r="C46" t="s">
+        <v>235</v>
+      </c>
+      <c r="D46" t="s">
+        <v>236</v>
+      </c>
+      <c r="E46" t="s">
+        <v>237</v>
+      </c>
+      <c r="F46" t="s">
+        <v>238</v>
+      </c>
+      <c r="G46" t="s">
+        <v>239</v>
+      </c>
+      <c r="H46" t="s">
+        <v>234</v>
+      </c>
+      <c r="I46" t="s">
+        <v>235</v>
+      </c>
+      <c r="J46" t="s">
+        <v>236</v>
+      </c>
+      <c r="K46" t="s">
+        <v>237</v>
+      </c>
+      <c r="L46" t="s">
+        <v>238</v>
+      </c>
+      <c r="M46" t="s">
+        <v>239</v>
+      </c>
+      <c r="N46" t="s">
+        <v>241</v>
+      </c>
+      <c r="O46" t="s">
+        <v>243</v>
+      </c>
+      <c r="P46" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>245</v>
+      </c>
+      <c r="R46" t="s">
+        <v>242</v>
+      </c>
+      <c r="S46" t="s">
+        <v>246</v>
+      </c>
+      <c r="T46" t="s">
+        <v>241</v>
+      </c>
+      <c r="U46" t="s">
+        <v>243</v>
+      </c>
+      <c r="V46" t="s">
+        <v>244</v>
+      </c>
+      <c r="W46" t="s">
+        <v>245</v>
+      </c>
+      <c r="X46" t="s">
+        <v>242</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>246</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4289,15 +4510,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59AB176E-27A4-4AEF-B4A1-CFE70075B06B}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:Z51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="A1:J24"/>
+      <selection activeCell="O16" sqref="O16:R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>226</v>
       </c>
@@ -4320,7 +4541,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>226</v>
       </c>
@@ -4343,7 +4564,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>226</v>
       </c>
@@ -4366,7 +4587,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>226</v>
       </c>
@@ -4392,7 +4613,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>226</v>
       </c>
@@ -4421,7 +4642,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>226</v>
       </c>
@@ -4447,7 +4668,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>226</v>
       </c>
@@ -4467,7 +4688,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>226</v>
       </c>
@@ -4496,7 +4717,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>226</v>
       </c>
@@ -4528,7 +4749,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>226</v>
       </c>
@@ -4556,8 +4777,44 @@
       <c r="J10" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>226</v>
       </c>
@@ -4582,8 +4839,44 @@
       <c r="J11" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>-1.47</v>
+      </c>
+      <c r="P11">
+        <v>-0.45</v>
+      </c>
+      <c r="Q11">
+        <v>-8.0000000000000016E-2</v>
+      </c>
+      <c r="R11">
+        <v>-2.39</v>
+      </c>
+      <c r="S11">
+        <v>-0.12000000000000001</v>
+      </c>
+      <c r="T11">
+        <v>-2.76</v>
+      </c>
+      <c r="U11">
+        <v>-3.2800000000000002</v>
+      </c>
+      <c r="V11">
+        <v>-3.29</v>
+      </c>
+      <c r="W11">
+        <v>-0.52</v>
+      </c>
+      <c r="X11">
+        <v>-2.59</v>
+      </c>
+      <c r="Y11">
+        <v>-2.17</v>
+      </c>
+      <c r="Z11">
+        <v>-3.5000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>226</v>
       </c>
@@ -4606,7 +4899,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>226</v>
       </c>
@@ -4629,7 +4922,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>226</v>
       </c>
@@ -4649,7 +4942,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>226</v>
       </c>
@@ -4678,7 +4971,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>226</v>
       </c>
@@ -4700,8 +4993,20 @@
       <c r="J16" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P16">
+        <v>-1.47</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R16">
+        <v>-3.2800000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>226</v>
       </c>
@@ -4726,8 +5031,20 @@
       <c r="J17" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P17">
+        <v>-0.45</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R17">
+        <v>-3.29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>226</v>
       </c>
@@ -4749,8 +5066,20 @@
       <c r="J18" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P18">
+        <v>-8.0000000000000016E-2</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R18">
+        <v>-0.52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>226</v>
       </c>
@@ -4772,8 +5101,20 @@
       <c r="J19" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P19">
+        <v>-2.39</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R19">
+        <v>-2.59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>226</v>
       </c>
@@ -4795,8 +5136,20 @@
       <c r="J20" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P20">
+        <v>-0.12000000000000001</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R20">
+        <v>-2.17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>226</v>
       </c>
@@ -4821,8 +5174,20 @@
       <c r="J21" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="O21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P21">
+        <v>-2.76</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R21">
+        <v>-3.5000000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>226</v>
       </c>
@@ -4848,7 +5213,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>226</v>
       </c>
@@ -4874,7 +5239,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>226</v>
       </c>
@@ -4898,6 +5263,389 @@
       </c>
       <c r="J24" t="s">
         <v>225</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="e">
+        <f>B16*B13</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C33" s="4" t="e">
+        <f t="shared" ref="C33:Y33" si="0">C16*C13</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D33" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E33" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F33" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O33" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="4" t="e">
+        <f>#REF!*Q13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R33" s="4" t="e">
+        <f>#REF!*R13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37" t="s">
+        <v>232</v>
+      </c>
+      <c r="F37" t="s">
+        <v>229</v>
+      </c>
+      <c r="G37" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>342</v>
+      </c>
+      <c r="D38" s="6">
+        <v>424</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38">
+        <v>163.80000000000001</v>
+      </c>
+      <c r="H38" s="7">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>345</v>
+      </c>
+      <c r="D39" s="7">
+        <v>430</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39">
+        <v>223.20000000000002</v>
+      </c>
+      <c r="H39" s="7">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>225.5</v>
+      </c>
+      <c r="D40" s="7">
+        <v>278</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40">
+        <v>254.1</v>
+      </c>
+      <c r="H40" s="7">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <v>247.5</v>
+      </c>
+      <c r="D41" s="7">
+        <v>347</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41">
+        <v>165</v>
+      </c>
+      <c r="H41" s="7">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>348</v>
+      </c>
+      <c r="D42" s="7">
+        <v>369</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42">
+        <v>150</v>
+      </c>
+      <c r="H42" s="7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43">
+        <v>177</v>
+      </c>
+      <c r="D43" s="7">
+        <v>246</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43">
+        <v>80.5</v>
+      </c>
+      <c r="H43" s="7">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44">
+        <v>350</v>
+      </c>
+      <c r="D44" s="7">
+        <v>395</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44">
+        <v>162</v>
+      </c>
+      <c r="H44" s="7">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>338.40000000000003</v>
+      </c>
+      <c r="D45" s="7">
+        <v>363</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45">
+        <v>180</v>
+      </c>
+      <c r="H45" s="7">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46">
+        <v>289.79999999999995</v>
+      </c>
+      <c r="D46" s="7">
+        <v>330</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46">
+        <v>192.5</v>
+      </c>
+      <c r="H46" s="7">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>234</v>
+      </c>
+      <c r="D47" s="7">
+        <v>341</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F47">
+        <v>235.6</v>
+      </c>
+      <c r="H47" s="7">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48">
+        <v>200</v>
+      </c>
+      <c r="D48" s="7">
+        <v>241</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F48">
+        <v>233.6</v>
+      </c>
+      <c r="H48" s="7">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49">
+        <v>226.3</v>
+      </c>
+      <c r="D49" s="7">
+        <v>331</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49">
+        <v>225</v>
+      </c>
+      <c r="H49" s="7">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B50">
+        <v>2740</v>
+      </c>
+      <c r="C50">
+        <v>3560</v>
+      </c>
+      <c r="D50">
+        <f>SUM(D38:D49)-D42-D47</f>
+        <v>3385</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F50">
+        <f>SUM(F38:F49)</f>
+        <v>2265.2999999999997</v>
+      </c>
+      <c r="G50">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <f>(D50-C50)/C50</f>
+        <v>-4.9157303370786519E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4907,23 +5655,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="fc8400a0-1a4f-4a7a-b485-adeb34e513bd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010081BE85D0812D9240B3A14D4E86FBD526" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="844c5fe439c283c57054fe603be8f4f0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fc8400a0-1a4f-4a7a-b485-adeb34e513bd" xmlns:ns4="f8e76daf-932e-4eb3-bd51-a2b94da941c5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5bfb24005f79649d2d34abed6e4c7d87" ns3:_="" ns4:_="">
     <xsd:import namespace="fc8400a0-1a4f-4a7a-b485-adeb34e513bd"/>
@@ -5158,10 +5889,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="fc8400a0-1a4f-4a7a-b485-adeb34e513bd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD85D50E-4653-4992-BCE8-249F2A1C10E6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17420F09-E15D-430F-A548-6FE9174B4D1D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fc8400a0-1a4f-4a7a-b485-adeb34e513bd"/>
+    <ds:schemaRef ds:uri="f8e76daf-932e-4eb3-bd51-a2b94da941c5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5184,20 +5943,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17420F09-E15D-430F-A548-6FE9174B4D1D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD85D50E-4653-4992-BCE8-249F2A1C10E6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="fc8400a0-1a4f-4a7a-b485-adeb34e513bd"/>
-    <ds:schemaRef ds:uri="f8e76daf-932e-4eb3-bd51-a2b94da941c5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>